<commit_message>
script for running with macro define
</commit_message>
<xml_diff>
--- a/project3/Workbook1.xlsx
+++ b/project3/Workbook1.xlsx
@@ -526,11 +526,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1671535456"/>
-        <c:axId val="-1636285088"/>
+        <c:axId val="-1941130576"/>
+        <c:axId val="-1941128704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1671535456"/>
+        <c:axId val="-1941130576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,7 +572,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1636285088"/>
+        <c:crossAx val="-1941128704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -580,7 +580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1636285088"/>
+        <c:axId val="-1941128704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +631,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1671535456"/>
+        <c:crossAx val="-1941130576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1259,16 +1259,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1553,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R4"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1817,6 +1817,179 @@
         <v>184.65259900000001</v>
       </c>
     </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>8</v>
+      </c>
+      <c r="K12">
+        <v>9</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <v>11</v>
+      </c>
+      <c r="N12">
+        <v>12</v>
+      </c>
+      <c r="O12">
+        <v>13</v>
+      </c>
+      <c r="P12">
+        <v>14</v>
+      </c>
+      <c r="Q12">
+        <v>15</v>
+      </c>
+      <c r="R12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>179.87795299999999</v>
+      </c>
+      <c r="C13">
+        <v>183.35587100000001</v>
+      </c>
+      <c r="D13">
+        <v>176.681567</v>
+      </c>
+      <c r="E13">
+        <v>177.056175</v>
+      </c>
+      <c r="F13">
+        <v>181.25053800000001</v>
+      </c>
+      <c r="G13">
+        <v>178.07139799999999</v>
+      </c>
+      <c r="H13">
+        <v>179.26929799999999</v>
+      </c>
+      <c r="I13">
+        <v>185.13461599999999</v>
+      </c>
+      <c r="J13">
+        <v>168.26872499999999</v>
+      </c>
+      <c r="K13">
+        <v>169.01170400000001</v>
+      </c>
+      <c r="L13">
+        <v>172.56851</v>
+      </c>
+      <c r="M13">
+        <v>181.375461</v>
+      </c>
+      <c r="N13">
+        <v>176.92695599999999</v>
+      </c>
+      <c r="O13">
+        <v>176.48434399999999</v>
+      </c>
+      <c r="P13">
+        <v>176.464879</v>
+      </c>
+      <c r="Q13">
+        <v>182.13941</v>
+      </c>
+      <c r="R13">
+        <v>178.56106600000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>34.884045</v>
+      </c>
+      <c r="C14">
+        <v>34.712730000000001</v>
+      </c>
+      <c r="D14">
+        <v>40.416818999999997</v>
+      </c>
+      <c r="E14">
+        <v>46.175725999999997</v>
+      </c>
+      <c r="F14">
+        <v>48.567855000000002</v>
+      </c>
+      <c r="G14">
+        <v>44.938367</v>
+      </c>
+      <c r="H14">
+        <v>46.302512999999998</v>
+      </c>
+      <c r="I14">
+        <v>71.035340000000005</v>
+      </c>
+      <c r="J14">
+        <v>64.556528999999998</v>
+      </c>
+      <c r="K14">
+        <v>65.428647999999995</v>
+      </c>
+      <c r="L14">
+        <v>66.771720999999999</v>
+      </c>
+      <c r="M14">
+        <v>63.314881999999997</v>
+      </c>
+      <c r="N14">
+        <v>68.232256000000007</v>
+      </c>
+      <c r="O14">
+        <v>69.510092999999998</v>
+      </c>
+      <c r="P14">
+        <v>69.109575000000007</v>
+      </c>
+      <c r="Q14">
+        <v>73.742369999999994</v>
+      </c>
+      <c r="R14">
+        <v>69.445167999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>71.747335000000007</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
results dont match textbook
</commit_message>
<xml_diff>
--- a/project3/Workbook1.xlsx
+++ b/project3/Workbook1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,63 +177,60 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$R$1</c:f>
+              <c:f>Sheet1!$B$13:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>183.686777</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>181.108566</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>177.716959</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0</c:v>
+                  <c:v>177.304965</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0</c:v>
+                  <c:v>168.82481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.0</c:v>
+                  <c:v>177.507178</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0</c:v>
+                  <c:v>173.032084</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0</c:v>
+                  <c:v>179.176951</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.0</c:v>
+                  <c:v>183.147667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.0</c:v>
+                  <c:v>182.523386</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.0</c:v>
+                  <c:v>176.854988</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.0</c:v>
+                  <c:v>181.702553</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.0</c:v>
+                  <c:v>169.251991</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12.0</c:v>
+                  <c:v>180.286565</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13.0</c:v>
+                  <c:v>180.484239</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.0</c:v>
+                  <c:v>181.258751</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>16.0</c:v>
+                  <c:v>182.922368</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -269,63 +266,60 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$R$2</c:f>
+              <c:f>Sheet1!$B$14:$R$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>36.716077</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>169.229077</c:v>
+                  <c:v>40.835036</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>169.751908</c:v>
+                  <c:v>52.904874</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>174.359556</c:v>
+                  <c:v>65.69018199999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>168.505483</c:v>
+                  <c:v>61.632617</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>166.953967</c:v>
+                  <c:v>58.805628</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>167.341611</c:v>
+                  <c:v>75.489645</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>170.529879</c:v>
+                  <c:v>79.27558000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>174.29118</c:v>
+                  <c:v>73.61236100000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>169.765596</c:v>
+                  <c:v>75.478819</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>169.896109</c:v>
+                  <c:v>77.064164</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>168.73223</c:v>
+                  <c:v>65.766866</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>170.053567</c:v>
+                  <c:v>72.812927</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>167.441082</c:v>
+                  <c:v>84.86659</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>168.570104</c:v>
+                  <c:v>73.277118</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>170.739516</c:v>
+                  <c:v>73.43357</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>169.833351</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>170.364281</c:v>
+                  <c:v>79.751017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -361,155 +355,60 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$R$3</c:f>
+              <c:f>Sheet1!$B$15:$R$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>67.079429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.014078</c:v>
+                  <c:v>60.90134</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47.747796</c:v>
+                  <c:v>67.68888200000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.996909</c:v>
+                  <c:v>75.971101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.925043</c:v>
+                  <c:v>74.440348</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45.960793</c:v>
+                  <c:v>69.955264</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62.651342</c:v>
+                  <c:v>69.014541</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60.428803</c:v>
+                  <c:v>77.50390899999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>111.827741</c:v>
+                  <c:v>80.132058</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>110.190105</c:v>
+                  <c:v>77.76337</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>109.713182</c:v>
+                  <c:v>74.963783</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>126.918049</c:v>
+                  <c:v>79.803683</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>121.674484</c:v>
+                  <c:v>76.69138</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>126.376716</c:v>
+                  <c:v>93.907295</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>121.955309</c:v>
+                  <c:v>91.550988</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>112.373755</c:v>
+                  <c:v>92.38600700000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>146.314877</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>142.817868</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$A$4:$R$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64.969554</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66.914249</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68.543619</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>69.905505</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>66.887507</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70.789068</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>73.351292</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>111.055892</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>110.912393</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>104.721088</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>103.776155</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>111.39672</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>112.730675</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>111.849004</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>111.720921</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>165.966151</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>152.739381</c:v>
+                  <c:v>97.273189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -526,11 +425,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1941130576"/>
-        <c:axId val="-1941128704"/>
+        <c:axId val="1969963520"/>
+        <c:axId val="1963360864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1941130576"/>
+        <c:axId val="1969963520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,7 +471,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1941128704"/>
+        <c:crossAx val="1963360864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -580,7 +479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1941128704"/>
+        <c:axId val="1963360864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +499,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -631,7 +529,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1941130576"/>
+        <c:crossAx val="1969963520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1259,20 +1157,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>641350</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1555,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1875,55 +1773,55 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>179.87795299999999</v>
+        <v>183.68677700000001</v>
       </c>
       <c r="C13">
-        <v>183.35587100000001</v>
+        <v>181.108566</v>
       </c>
       <c r="D13">
-        <v>176.681567</v>
+        <v>177.716959</v>
       </c>
       <c r="E13">
-        <v>177.056175</v>
+        <v>177.30496500000001</v>
       </c>
       <c r="F13">
-        <v>181.25053800000001</v>
+        <v>168.82481000000001</v>
       </c>
       <c r="G13">
-        <v>178.07139799999999</v>
+        <v>177.50717800000001</v>
       </c>
       <c r="H13">
-        <v>179.26929799999999</v>
+        <v>173.032084</v>
       </c>
       <c r="I13">
-        <v>185.13461599999999</v>
+        <v>179.176951</v>
       </c>
       <c r="J13">
-        <v>168.26872499999999</v>
+        <v>183.14766700000001</v>
       </c>
       <c r="K13">
-        <v>169.01170400000001</v>
+        <v>182.52338599999999</v>
       </c>
       <c r="L13">
-        <v>172.56851</v>
+        <v>176.85498799999999</v>
       </c>
       <c r="M13">
-        <v>181.375461</v>
+        <v>181.70255299999999</v>
       </c>
       <c r="N13">
-        <v>176.92695599999999</v>
+        <v>169.251991</v>
       </c>
       <c r="O13">
-        <v>176.48434399999999</v>
+        <v>180.286565</v>
       </c>
       <c r="P13">
-        <v>176.464879</v>
+        <v>180.484239</v>
       </c>
       <c r="Q13">
-        <v>182.13941</v>
+        <v>181.25875099999999</v>
       </c>
       <c r="R13">
-        <v>178.56106600000001</v>
+        <v>182.92236800000001</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1931,55 +1829,55 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>34.884045</v>
+        <v>36.716076999999999</v>
       </c>
       <c r="C14">
-        <v>34.712730000000001</v>
+        <v>40.835036000000002</v>
       </c>
       <c r="D14">
-        <v>40.416818999999997</v>
+        <v>52.904874</v>
       </c>
       <c r="E14">
-        <v>46.175725999999997</v>
+        <v>65.690181999999993</v>
       </c>
       <c r="F14">
-        <v>48.567855000000002</v>
+        <v>61.632617000000003</v>
       </c>
       <c r="G14">
-        <v>44.938367</v>
+        <v>58.805627999999999</v>
       </c>
       <c r="H14">
-        <v>46.302512999999998</v>
+        <v>75.489644999999996</v>
       </c>
       <c r="I14">
-        <v>71.035340000000005</v>
+        <v>79.275580000000005</v>
       </c>
       <c r="J14">
-        <v>64.556528999999998</v>
+        <v>73.612361000000007</v>
       </c>
       <c r="K14">
-        <v>65.428647999999995</v>
+        <v>75.478819000000001</v>
       </c>
       <c r="L14">
-        <v>66.771720999999999</v>
+        <v>77.064164000000005</v>
       </c>
       <c r="M14">
-        <v>63.314881999999997</v>
+        <v>65.766865999999993</v>
       </c>
       <c r="N14">
-        <v>68.232256000000007</v>
+        <v>72.812927000000002</v>
       </c>
       <c r="O14">
-        <v>69.510092999999998</v>
+        <v>84.866590000000002</v>
       </c>
       <c r="P14">
-        <v>69.109575000000007</v>
+        <v>73.277118000000002</v>
       </c>
       <c r="Q14">
-        <v>73.742369999999994</v>
+        <v>73.433570000000003</v>
       </c>
       <c r="R14">
-        <v>69.445167999999995</v>
+        <v>79.751017000000004</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -1987,7 +1885,55 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>71.747335000000007</v>
+        <v>67.079429000000005</v>
+      </c>
+      <c r="C15">
+        <v>60.901339999999998</v>
+      </c>
+      <c r="D15">
+        <v>67.688882000000007</v>
+      </c>
+      <c r="E15">
+        <v>75.971101000000004</v>
+      </c>
+      <c r="F15">
+        <v>74.440348</v>
+      </c>
+      <c r="G15">
+        <v>69.955264</v>
+      </c>
+      <c r="H15">
+        <v>69.014540999999994</v>
+      </c>
+      <c r="I15">
+        <v>77.503908999999993</v>
+      </c>
+      <c r="J15">
+        <v>80.132058000000001</v>
+      </c>
+      <c r="K15">
+        <v>77.763369999999995</v>
+      </c>
+      <c r="L15">
+        <v>74.963783000000006</v>
+      </c>
+      <c r="M15">
+        <v>79.803683000000007</v>
+      </c>
+      <c r="N15">
+        <v>76.691379999999995</v>
+      </c>
+      <c r="O15">
+        <v>93.907295000000005</v>
+      </c>
+      <c r="P15">
+        <v>91.550988000000004</v>
+      </c>
+      <c r="Q15">
+        <v>92.386007000000006</v>
+      </c>
+      <c r="R15">
+        <v>97.273189000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use +2.0f instead of rand()
</commit_message>
<xml_diff>
--- a/project3/Workbook1.xlsx
+++ b/project3/Workbook1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>fix#2</t>
   </si>
   <si>
     <t xml:space="preserve">            NUMPAD
 NUMT</t>
+  </si>
+  <si>
+    <t>fix #1</t>
+  </si>
+  <si>
+    <t>fix #2</t>
   </si>
 </sst>
 </file>
@@ -182,55 +188,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>183.686777</c:v>
+                  <c:v>344.711692</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>181.108566</c:v>
+                  <c:v>338.592808</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>177.716959</c:v>
+                  <c:v>325.934617</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>177.304965</c:v>
+                  <c:v>344.317047</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>168.82481</c:v>
+                  <c:v>325.277299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>177.507178</c:v>
+                  <c:v>318.013054</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>173.032084</c:v>
+                  <c:v>331.394675</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>179.176951</c:v>
+                  <c:v>339.19289</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>183.147667</c:v>
+                  <c:v>330.747986</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>182.523386</c:v>
+                  <c:v>328.774329</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>176.854988</c:v>
+                  <c:v>324.899484</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>181.702553</c:v>
+                  <c:v>331.76574</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>169.251991</c:v>
+                  <c:v>330.332811</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>180.286565</c:v>
+                  <c:v>321.310949</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>180.484239</c:v>
+                  <c:v>325.504939</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>181.258751</c:v>
+                  <c:v>342.430572</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>182.922368</c:v>
+                  <c:v>328.498924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -271,55 +277,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>36.716077</c:v>
+                  <c:v>337.518564</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.835036</c:v>
+                  <c:v>365.607319</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.904874</c:v>
+                  <c:v>409.064878</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65.69018199999999</c:v>
+                  <c:v>682.430817</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61.632617</c:v>
+                  <c:v>629.653533</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58.805628</c:v>
+                  <c:v>661.288189</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>75.489645</c:v>
+                  <c:v>632.721176</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79.27558000000001</c:v>
+                  <c:v>702.827121</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>73.61236100000001</c:v>
+                  <c:v>645.598631</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>75.478819</c:v>
+                  <c:v>664.451827</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>77.064164</c:v>
+                  <c:v>625.25401</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>65.766866</c:v>
+                  <c:v>664.551179</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>72.812927</c:v>
+                  <c:v>641.724957</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>84.86659</c:v>
+                  <c:v>651.253663</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>73.277118</c:v>
+                  <c:v>629.84191</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>73.43357</c:v>
+                  <c:v>690.405096</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>79.751017</c:v>
+                  <c:v>643.469588</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -360,55 +366,410 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>67.079429</c:v>
+                  <c:v>333.736598</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60.90134</c:v>
+                  <c:v>372.415206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.68888200000001</c:v>
+                  <c:v>413.052458</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.971101</c:v>
+                  <c:v>593.788967</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.440348</c:v>
+                  <c:v>545.8813259999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69.955264</c:v>
+                  <c:v>534.730763</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69.014541</c:v>
+                  <c:v>536.0565</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77.50390899999999</c:v>
+                  <c:v>622.6650059999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80.132058</c:v>
+                  <c:v>533.27645</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>77.76337</c:v>
+                  <c:v>571.23272</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>74.963783</c:v>
+                  <c:v>539.803781</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>79.803683</c:v>
+                  <c:v>617.426874</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>76.69138</c:v>
+                  <c:v>586.579072</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>93.907295</c:v>
+                  <c:v>907.194049</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>91.550988</c:v>
+                  <c:v>949.64507</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>92.38600700000001</c:v>
+                  <c:v>1065.530103</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>97.273189</c:v>
+                  <c:v>982.197668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$R$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$R$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$R$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>338.980178</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$R$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>700.905921</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$20:$R$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1055.576079</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1055.576079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -425,11 +786,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1969963520"/>
-        <c:axId val="1963360864"/>
+        <c:axId val="1011700640"/>
+        <c:axId val="1010238032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1969963520"/>
+        <c:axId val="1011700640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,7 +832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1963360864"/>
+        <c:crossAx val="1010238032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -479,7 +840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1963360864"/>
+        <c:axId val="1010238032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,7 +890,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1969963520"/>
+        <c:crossAx val="1011700640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1157,20 +1518,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1451,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:R15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1716,6 +2077,9 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
       <c r="B12">
         <v>0</v>
       </c>
@@ -1773,55 +2137,55 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>183.68677700000001</v>
+        <v>344.71169200000003</v>
       </c>
       <c r="C13">
-        <v>181.108566</v>
+        <v>338.59280799999999</v>
       </c>
       <c r="D13">
-        <v>177.716959</v>
+        <v>325.934617</v>
       </c>
       <c r="E13">
-        <v>177.30496500000001</v>
+        <v>344.317047</v>
       </c>
       <c r="F13">
-        <v>168.82481000000001</v>
+        <v>325.27729900000003</v>
       </c>
       <c r="G13">
-        <v>177.50717800000001</v>
+        <v>318.01305400000001</v>
       </c>
       <c r="H13">
-        <v>173.032084</v>
+        <v>331.39467500000001</v>
       </c>
       <c r="I13">
-        <v>179.176951</v>
+        <v>339.19288999999998</v>
       </c>
       <c r="J13">
-        <v>183.14766700000001</v>
+        <v>330.74798600000003</v>
       </c>
       <c r="K13">
-        <v>182.52338599999999</v>
+        <v>328.77432900000002</v>
       </c>
       <c r="L13">
-        <v>176.85498799999999</v>
+        <v>324.89948399999997</v>
       </c>
       <c r="M13">
-        <v>181.70255299999999</v>
+        <v>331.76573999999999</v>
       </c>
       <c r="N13">
-        <v>169.251991</v>
+        <v>330.33281099999999</v>
       </c>
       <c r="O13">
-        <v>180.286565</v>
+        <v>321.31094899999999</v>
       </c>
       <c r="P13">
-        <v>180.484239</v>
+        <v>325.50493899999998</v>
       </c>
       <c r="Q13">
-        <v>181.25875099999999</v>
+        <v>342.43057199999998</v>
       </c>
       <c r="R13">
-        <v>182.92236800000001</v>
+        <v>328.49892399999999</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1829,55 +2193,55 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>36.716076999999999</v>
+        <v>337.51856400000003</v>
       </c>
       <c r="C14">
-        <v>40.835036000000002</v>
+        <v>365.60731900000002</v>
       </c>
       <c r="D14">
-        <v>52.904874</v>
+        <v>409.06487800000002</v>
       </c>
       <c r="E14">
-        <v>65.690181999999993</v>
+        <v>682.43081700000005</v>
       </c>
       <c r="F14">
-        <v>61.632617000000003</v>
+        <v>629.65353300000004</v>
       </c>
       <c r="G14">
-        <v>58.805627999999999</v>
+        <v>661.28818899999999</v>
       </c>
       <c r="H14">
-        <v>75.489644999999996</v>
+        <v>632.72117600000001</v>
       </c>
       <c r="I14">
-        <v>79.275580000000005</v>
+        <v>702.82712100000003</v>
       </c>
       <c r="J14">
-        <v>73.612361000000007</v>
+        <v>645.59863099999995</v>
       </c>
       <c r="K14">
-        <v>75.478819000000001</v>
+        <v>664.45182699999998</v>
       </c>
       <c r="L14">
-        <v>77.064164000000005</v>
+        <v>625.25400999999999</v>
       </c>
       <c r="M14">
-        <v>65.766865999999993</v>
+        <v>664.55117900000005</v>
       </c>
       <c r="N14">
-        <v>72.812927000000002</v>
+        <v>641.72495700000002</v>
       </c>
       <c r="O14">
-        <v>84.866590000000002</v>
+        <v>651.25366299999996</v>
       </c>
       <c r="P14">
-        <v>73.277118000000002</v>
+        <v>629.84190999999998</v>
       </c>
       <c r="Q14">
-        <v>73.433570000000003</v>
+        <v>690.40509599999996</v>
       </c>
       <c r="R14">
-        <v>79.751017000000004</v>
+        <v>643.46958800000004</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -1885,55 +2249,228 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>67.079429000000005</v>
+        <v>333.73659800000001</v>
       </c>
       <c r="C15">
-        <v>60.901339999999998</v>
+        <v>372.41520600000001</v>
       </c>
       <c r="D15">
-        <v>67.688882000000007</v>
+        <v>413.052458</v>
       </c>
       <c r="E15">
-        <v>75.971101000000004</v>
+        <v>593.78896699999996</v>
       </c>
       <c r="F15">
-        <v>74.440348</v>
+        <v>545.88132599999994</v>
       </c>
       <c r="G15">
-        <v>69.955264</v>
+        <v>534.73076300000002</v>
       </c>
       <c r="H15">
-        <v>69.014540999999994</v>
+        <v>536.05650000000003</v>
       </c>
       <c r="I15">
-        <v>77.503908999999993</v>
+        <v>622.66500599999995</v>
       </c>
       <c r="J15">
-        <v>80.132058000000001</v>
+        <v>533.27644999999995</v>
       </c>
       <c r="K15">
-        <v>77.763369999999995</v>
+        <v>571.23271999999997</v>
       </c>
       <c r="L15">
-        <v>74.963783000000006</v>
+        <v>539.80378099999996</v>
       </c>
       <c r="M15">
-        <v>79.803683000000007</v>
+        <v>617.426874</v>
       </c>
       <c r="N15">
-        <v>76.691379999999995</v>
+        <v>586.579072</v>
       </c>
       <c r="O15">
-        <v>93.907295000000005</v>
+        <v>907.19404899999995</v>
       </c>
       <c r="P15">
-        <v>91.550988000000004</v>
+        <v>949.64507000000003</v>
       </c>
       <c r="Q15">
-        <v>92.386007000000006</v>
+        <v>1065.5301030000001</v>
       </c>
       <c r="R15">
-        <v>97.273189000000002</v>
+        <v>982.19766800000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="C18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="D18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="E18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="F18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="G18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="H18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="I18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="J18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="K18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="L18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="M18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="N18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="O18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="P18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="Q18">
+        <v>338.98017800000002</v>
+      </c>
+      <c r="R18">
+        <v>338.98017800000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="C19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="D19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="E19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="F19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="G19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="H19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="I19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="J19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="K19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="L19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="M19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="N19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="O19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="P19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="Q19">
+        <v>700.90592100000003</v>
+      </c>
+      <c r="R19">
+        <v>700.90592100000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="C20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="D20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="E20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="F20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="G20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="H20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="I20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="J20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="K20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="L20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="M20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="N20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="O20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="P20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="Q20">
+        <v>1055.5760789999999</v>
+      </c>
+      <c r="R20">
+        <v>1055.5760789999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>